<commit_message>
Revert "Merge pull request #20 from advait22/advait"
This reverts commit 4bbfadd78ab635c26f1966edfdb35bfedd0ac688, reversing
changes made to 435ac6e47aa374d767e3322aac0eec486ff59d24.
</commit_message>
<xml_diff>
--- a/project-data/rm-category-type-py-compatible.xlsx
+++ b/project-data/rm-category-type-py-compatible.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsharma13/Google Drive/Mission Data Science [2019-2020]/Semester 3/MAST90106/MAST90106/project-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942E2DED-82D3-5C45-AA91-28E563C62631}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A07841-F17F-1844-AAF3-47CF3267ECA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2574,13 +2574,13 @@
     <t>A non-reportable workstation.</t>
   </si>
   <si>
-    <t xml:space="preserve">Room Category </t>
-  </si>
-  <si>
     <t>Room Type</t>
   </si>
   <si>
     <t>Room Type Abbreviation</t>
+  </si>
+  <si>
+    <t>Room Category</t>
   </si>
 </sst>
 </file>
@@ -3089,7 +3089,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3104,13 +3104,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>848</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>849</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>

</xml_diff>